<commit_message>
Updated code and labeling data
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Library/CloudStorage/Box-Box/LatvianStarling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C379C591-4217-4E48-BF33-98E4CAEFB95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194DC827-0431-5741-B938-9167D454584B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42680" yWindow="1560" windowWidth="27740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9920" yWindow="22100" windowWidth="27720" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>mass</t>
   </si>
@@ -184,13 +184,16 @@
   </si>
   <si>
     <t>usable</t>
+  </si>
+  <si>
+    <t>Possible exploratory flight on the 2021-01-19.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,6 +345,11 @@
       <color rgb="FFAD0000"/>
       <name val="Var(--bs-font-monospace)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -524,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -639,6 +647,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -685,12 +706,18 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -739,16 +766,7 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -763,7 +781,16 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yy"/>
@@ -847,17 +874,17 @@
     <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust"/>
     <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon"/>
     <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="0"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="10"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="8"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="7"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="6"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1165,11 +1192,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI17"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB8" sqref="AB8"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1332,28 +1359,28 @@
         <v>-11</v>
       </c>
       <c r="H2">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I2">
         <v>30</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K2">
         <v>100</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O2">
         <v>0.9</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q2">
         <v>1.4</v>
@@ -1382,10 +1409,10 @@
         <v>0.1</v>
       </c>
       <c r="AA2" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB2" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC2" s="3">
         <v>100</v>
@@ -1424,28 +1451,28 @@
         <v>-11</v>
       </c>
       <c r="H3">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I3">
         <v>30</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K3">
         <v>100</v>
       </c>
       <c r="L3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O3">
         <v>0.9</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q3">
         <v>1.4</v>
@@ -1459,21 +1486,21 @@
       <c r="T3" s="1">
         <v>43976</v>
       </c>
-      <c r="U3" s="1"/>
+      <c r="U3" s="1">
+        <v>43995</v>
+      </c>
       <c r="V3" s="1"/>
-      <c r="W3" s="1">
-        <v>44179</v>
-      </c>
+      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="3">
         <v>0.1</v>
       </c>
       <c r="AA3" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB3" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC3" s="3">
         <v>100</v>
@@ -1511,28 +1538,28 @@
         <v>-11</v>
       </c>
       <c r="H4">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I4">
         <v>30</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K4">
         <v>100</v>
       </c>
       <c r="L4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O4">
         <v>0.9</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q4">
         <v>1.4</v>
@@ -1561,10 +1588,10 @@
         <v>0.1</v>
       </c>
       <c r="AA4" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB4" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC4" s="3">
         <v>100</v>
@@ -1602,28 +1629,28 @@
         <v>-11</v>
       </c>
       <c r="H5">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I5">
         <v>30</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <v>100</v>
       </c>
       <c r="L5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O5">
         <v>0.9</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q5">
         <v>1.4</v>
@@ -1652,10 +1679,10 @@
         <v>0.1</v>
       </c>
       <c r="AA5" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB5" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC5" s="3">
         <v>100</v>
@@ -1693,28 +1720,28 @@
         <v>-11</v>
       </c>
       <c r="H6">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I6">
         <v>30</v>
       </c>
       <c r="J6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>100</v>
       </c>
       <c r="L6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O6">
         <v>0.9</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q6">
         <v>1.4</v>
@@ -1728,7 +1755,9 @@
       <c r="T6" s="1">
         <v>43970</v>
       </c>
-      <c r="U6" s="1"/>
+      <c r="U6" s="1">
+        <v>44080</v>
+      </c>
       <c r="V6" s="1">
         <v>44269</v>
       </c>
@@ -1741,10 +1770,10 @@
         <v>0.1</v>
       </c>
       <c r="AA6" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB6" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC6" s="3">
         <v>100</v>
@@ -1782,28 +1811,28 @@
         <v>-11</v>
       </c>
       <c r="H7">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I7">
         <v>30</v>
       </c>
       <c r="J7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K7">
         <v>100</v>
       </c>
       <c r="L7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O7">
         <v>0.9</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q7">
         <v>1.4</v>
@@ -1832,10 +1861,10 @@
         <v>0.1</v>
       </c>
       <c r="AA7" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB7" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC7" s="3">
         <v>100</v>
@@ -1848,17 +1877,24 @@
       </c>
       <c r="AF7" t="s">
         <v>46</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>43972</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44569</v>
+      </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
@@ -1869,28 +1905,28 @@
         <v>-11</v>
       </c>
       <c r="H8">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I8">
         <v>30</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K8">
         <v>100</v>
       </c>
       <c r="L8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O8">
         <v>0.9</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q8">
         <v>1.4</v>
@@ -1901,20 +1937,28 @@
       <c r="S8">
         <v>57.276000000000003</v>
       </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="T8" s="1">
+        <v>43972</v>
+      </c>
+      <c r="U8" s="1">
+        <v>44041</v>
+      </c>
+      <c r="V8" s="1">
+        <v>44409</v>
+      </c>
+      <c r="W8" s="1">
+        <v>44448</v>
+      </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="3">
         <v>0.1</v>
       </c>
       <c r="AA8" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB8" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC8" s="3">
         <v>100</v>
@@ -1927,23 +1971,20 @@
       </c>
       <c r="AF8" t="s">
         <v>46</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>43972</v>
+        <v>43971</v>
       </c>
       <c r="D9" s="1">
-        <v>44569</v>
+        <v>44340</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -1955,28 +1996,28 @@
         <v>-11</v>
       </c>
       <c r="H9">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I9">
         <v>30</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <v>100</v>
       </c>
       <c r="L9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O9">
         <v>0.9</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q9">
         <v>1.4</v>
@@ -1988,12 +2029,16 @@
         <v>57.276000000000003</v>
       </c>
       <c r="T9" s="1">
-        <v>43972</v>
-      </c>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+        <v>43971</v>
+      </c>
+      <c r="U9" s="1">
+        <v>44135</v>
+      </c>
+      <c r="V9" s="1">
+        <v>44282</v>
+      </c>
       <c r="W9" s="1">
-        <v>44569</v>
+        <v>44340</v>
       </c>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
@@ -2001,10 +2046,10 @@
         <v>0.1</v>
       </c>
       <c r="AA9" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB9" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC9" s="3">
         <v>100</v>
@@ -2021,7 +2066,7 @@
     </row>
     <row r="10" spans="1:35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -2042,28 +2087,28 @@
         <v>-11</v>
       </c>
       <c r="H10">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I10">
         <v>30</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K10">
         <v>100</v>
       </c>
       <c r="L10">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O10">
         <v>0.9</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q10">
         <v>1.4</v>
@@ -2077,8 +2122,12 @@
       <c r="T10" s="1">
         <v>43971</v>
       </c>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+      <c r="U10" s="1">
+        <v>44135</v>
+      </c>
+      <c r="V10" s="1">
+        <v>44296</v>
+      </c>
       <c r="W10" s="1">
         <v>44344</v>
       </c>
@@ -2088,10 +2137,10 @@
         <v>0.1</v>
       </c>
       <c r="AA10" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB10" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC10" s="3">
         <v>100</v>
@@ -2104,23 +2153,20 @@
       </c>
       <c r="AF10" t="s">
         <v>46</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="D11" s="1">
-        <v>44340</v>
+        <v>44339</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -2132,28 +2178,28 @@
         <v>-11</v>
       </c>
       <c r="H11">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I11">
         <v>30</v>
       </c>
       <c r="J11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K11">
         <v>100</v>
       </c>
       <c r="L11">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="O11">
         <v>0.9</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>-7200</v>
       </c>
       <c r="Q11">
         <v>1.4</v>
@@ -2165,16 +2211,16 @@
         <v>57.276000000000003</v>
       </c>
       <c r="T11" s="1">
-        <v>43971</v>
+        <v>43972</v>
       </c>
       <c r="U11" s="1">
-        <v>44135</v>
+        <v>44142</v>
       </c>
       <c r="V11" s="1">
-        <v>44282</v>
+        <v>44281</v>
       </c>
       <c r="W11" s="1">
-        <v>44340</v>
+        <v>44339</v>
       </c>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -2182,10 +2228,10 @@
         <v>0.1</v>
       </c>
       <c r="AA11" s="3">
-        <v>0.9</v>
+        <v>0.99</v>
       </c>
       <c r="AB11" s="3">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="AC11" s="3">
         <v>100</v>
@@ -2202,188 +2248,128 @@
     </row>
     <row r="12" spans="1:35">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43971</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44344</v>
-      </c>
-      <c r="E12" s="3">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>60</v>
-      </c>
-      <c r="G12">
-        <v>-11</v>
-      </c>
-      <c r="H12">
-        <v>45</v>
-      </c>
-      <c r="I12">
-        <v>30</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12">
-        <v>100</v>
-      </c>
-      <c r="L12">
-        <v>30</v>
-      </c>
-      <c r="M12">
-        <v>2</v>
-      </c>
-      <c r="O12">
-        <v>0.9</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>1.4</v>
-      </c>
-      <c r="R12">
-        <v>23.111999999999998</v>
-      </c>
-      <c r="S12">
-        <v>57.276000000000003</v>
-      </c>
-      <c r="T12" s="1">
-        <v>43971</v>
-      </c>
-      <c r="U12" s="1">
-        <v>44135</v>
-      </c>
-      <c r="V12" s="1">
-        <v>44296</v>
-      </c>
-      <c r="W12" s="1">
-        <v>44344</v>
-      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="AA12" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="AB12" s="3">
-        <v>120</v>
-      </c>
-      <c r="AC12" s="3">
-        <v>100</v>
-      </c>
-      <c r="AD12" s="3">
-        <v>15</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>46</v>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AI12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="b">
+      <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>43971</v>
+      </c>
+      <c r="D13" s="7">
+        <v>44344</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>60</v>
+      </c>
+      <c r="G13" s="6">
+        <v>-11</v>
+      </c>
+      <c r="H13" s="6">
+        <v>48</v>
+      </c>
+      <c r="I13" s="6">
+        <v>30</v>
+      </c>
+      <c r="J13" s="6">
+        <v>2</v>
+      </c>
+      <c r="K13" s="6">
+        <v>100</v>
+      </c>
+      <c r="L13" s="6">
+        <v>20</v>
+      </c>
+      <c r="M13" s="6">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
-        <v>43972</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44339</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>60</v>
-      </c>
-      <c r="G13">
-        <v>-11</v>
-      </c>
-      <c r="H13">
+      <c r="N13" s="6"/>
+      <c r="O13" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="P13" s="8">
+        <v>-7200</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="R13" s="6">
+        <v>23.111999999999998</v>
+      </c>
+      <c r="S13" s="6">
+        <v>57.276000000000003</v>
+      </c>
+      <c r="T13" s="7">
+        <v>43971</v>
+      </c>
+      <c r="U13" s="7">
+        <v>44038</v>
+      </c>
+      <c r="V13" s="7">
+        <v>44271</v>
+      </c>
+      <c r="W13" s="7">
+        <v>44344</v>
+      </c>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>120</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>100</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>15</v>
+      </c>
+      <c r="AE13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I13">
-        <v>30</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <v>30</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-      <c r="O13">
-        <v>0.9</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>1.4</v>
-      </c>
-      <c r="R13">
-        <v>23.111999999999998</v>
-      </c>
-      <c r="S13">
-        <v>57.276000000000003</v>
-      </c>
-      <c r="T13" s="1">
-        <v>43972</v>
-      </c>
-      <c r="U13" s="1">
-        <v>44142</v>
-      </c>
-      <c r="V13" s="1">
-        <v>44281</v>
-      </c>
-      <c r="W13" s="1">
-        <v>44339</v>
-      </c>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="AA13" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="AB13" s="3">
-        <v>120</v>
-      </c>
-      <c r="AC13" s="3">
-        <v>100</v>
-      </c>
-      <c r="AD13" s="3">
-        <v>15</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF13" t="s">
+      <c r="AF13" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="AG13" s="6"/>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="17" spans="9:9">
-      <c r="I17" s="4"/>
+    <row r="16" spans="1:35">
+      <c r="I16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>